<commit_message>
Updating metadata and adding csv
</commit_message>
<xml_diff>
--- a/Non-50-magnification-files/non-50-magnification-metadata.xlsx
+++ b/Non-50-magnification-files/non-50-magnification-metadata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
   <si>
     <t xml:space="preserve">Filename</t>
   </si>
@@ -164,6 +164,15 @@
   </si>
   <si>
     <t xml:space="preserve">MHR.7198</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.0725513 pixels per μm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-p [1500,700,3,250]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Almost all bad due to debris and angle, two might be okay, but area seems overestimated on all objects, and neither avicularia on autozooid 1 are detected, even with confidence 0, strictness 1.00 or autofilter turned off.</t>
   </si>
   <si>
     <t xml:space="preserve">MHR.</t>
@@ -611,7 +620,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>47</v>
       </c>
@@ -621,15 +630,40 @@
       <c r="C9" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="D9" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="E9" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>60</v>
@@ -645,7 +679,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>60</v>
@@ -661,7 +695,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>60</v>

</xml_diff>